<commit_message>
Removed sapphire for the time being as it is no isotropic
</commit_message>
<xml_diff>
--- a/PDielec/MaterialsDataBase.xlsx
+++ b/PDielec/MaterialsDataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\home\Software\PDielec\PDielec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7327CD2-0FED-4C5B-83B7-B4056A884843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A4E05A-3A66-4A41-A80C-532258DCD360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="667" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" tabRatio="667" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -30485,8 +30485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H621"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75"/>
@@ -41176,7 +41176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36620115-7B2A-4542-9163-1157C9673F5F}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor updates to default database
</commit_message>
<xml_diff>
--- a/PDielec/MaterialsDataBase.xlsx
+++ b/PDielec/MaterialsDataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\home\Software\PDielec\PDielec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEED5C14-8BC1-425F-9F4A-0EE42EAA89CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFB0849-87DF-4396-BA76-67C7428FB79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" xr2:uid="{0AAABBAC-0EC7-4710-95BD-77FE6DEEE0A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="675" firstSheet="2" activeTab="9" xr2:uid="{0AAABBAC-0EC7-4710-95BD-77FE6DEEE0A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,12 @@
     <sheet name="kbr" sheetId="7" r:id="rId7"/>
     <sheet name="nujol" sheetId="8" r:id="rId8"/>
     <sheet name="Polypropylene" sheetId="9" r:id="rId9"/>
-    <sheet name="Water(25C)" sheetId="10" r:id="rId10"/>
-    <sheet name="Water(19C)" sheetId="11" r:id="rId11"/>
-    <sheet name="Silver" sheetId="12" r:id="rId12"/>
-    <sheet name="Fused Silica" sheetId="13" r:id="rId13"/>
-    <sheet name="PVC" sheetId="14" r:id="rId14"/>
+    <sheet name="Silicon" sheetId="15" r:id="rId10"/>
+    <sheet name="Water(25C)" sheetId="10" r:id="rId11"/>
+    <sheet name="Water(19C)" sheetId="11" r:id="rId12"/>
+    <sheet name="Silver" sheetId="12" r:id="rId13"/>
+    <sheet name="Fused Silica" sheetId="13" r:id="rId14"/>
+    <sheet name="PVC" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="43">
   <si>
     <t>Information</t>
   </si>
@@ -165,14 +166,17 @@
   <si>
     <t>1) X. Zhang, J. Qiu, X. Li, J. Zhao, L. Liu. Complex refractive indices measurements of polymers in visible and near-infrared bands, &lt;a href=\"https://doi.org/10.1364/AO.383831\"&gt;&lt;i&gt;Appl. Opt.&lt;/i&gt; &lt;b&gt;59&lt;/b&gt;, 2337-2344 (2020)&lt;/a&gt; (0.4-2 Âµm)&lt;br&gt;2) X. Zhang, J. Qiu, J. Zhao, X. Li, L. Liu. Complex refractive indices measurements of polymers in infrared bands, &lt;a href=\"https://doi.org/10.1016/j.jqsrt.2020.107063\"&gt;&lt;i&gt;J. Quant. Spectrosc. Radiat. Transf.&lt;/i&gt; &lt;b&gt;252&lt;/b&gt;, 107063 (2020)&lt;/a&gt; (2-20 Âµm)"</t>
   </si>
+  <si>
+    <t>D . F . Edwards, in Handbook of Optical Constants of Solids, edited by E. D. Palik (Academic, Orlando, 1985), pp. 547-569.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -220,8 +224,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F272EF3F-D9AE-4C8B-835E-2EB825164062}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -712,6 +716,99 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B879817-DB0B-4B3A-84E7-A7551823413C}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="2">
+        <v>3.42</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <f>MIN(A2:A618)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <f>MAX(A2:A618)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <f>COUNT(A2:A618)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C8F1AD-76E7-41FE-9838-E8BB2D87283B}">
   <dimension ref="A1:H172"/>
   <sheetViews>
@@ -3361,7 +3458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CE6550-E78D-4725-8926-CC7145BBFF2A}">
   <dimension ref="A1:H36"/>
   <sheetViews>
@@ -3959,7 +4056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583FF851-E030-4853-BD33-73679A7EFC1D}">
   <dimension ref="A1:H151"/>
   <sheetViews>
@@ -6283,7 +6380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389790FE-AA16-409F-98F5-59401C0123E9}">
   <dimension ref="A1:H203"/>
   <sheetViews>
@@ -9389,7 +9486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD1BA1-E705-4119-8F2D-870A4D09B5AF}">
   <dimension ref="A1:H621"/>
   <sheetViews>
@@ -19375,7 +19472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A58B27-5900-4BF7-B438-3F434021BD92}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>